<commit_message>
tested and working correctly
</commit_message>
<xml_diff>
--- a/multi.xlsx
+++ b/multi.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="C1:H93"/>
+  <dimension ref="C1:H126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1410,6 +1410,345 @@
         <v>353</v>
       </c>
     </row>
+    <row r="94">
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>2019-11-01</t>
+        </is>
+      </c>
+      <c r="D94" t="n">
+        <v>228</v>
+      </c>
+      <c r="E94" t="n">
+        <v>296</v>
+      </c>
+      <c r="F94" t="n">
+        <v>183</v>
+      </c>
+      <c r="G94" t="n">
+        <v>284</v>
+      </c>
+      <c r="H94" t="n">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>2019-11-02</t>
+        </is>
+      </c>
+      <c r="D95" t="n">
+        <v>228</v>
+      </c>
+      <c r="E95" t="n">
+        <v>296</v>
+      </c>
+      <c r="F95" t="n">
+        <v>178</v>
+      </c>
+      <c r="G95" t="n">
+        <v>282</v>
+      </c>
+      <c r="H95" t="n">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>2019-11-01</t>
+        </is>
+      </c>
+      <c r="D96" t="n">
+        <v>228</v>
+      </c>
+      <c r="E96" t="n">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>2019-11-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>2019-11-01</t>
+        </is>
+      </c>
+      <c r="D98" t="n">
+        <v>228</v>
+      </c>
+      <c r="E98" t="n">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>2019-11-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>2019-11-01</t>
+        </is>
+      </c>
+      <c r="D100" t="n">
+        <v>228</v>
+      </c>
+      <c r="E100" t="n">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>2019-11-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>2019-11-01</t>
+        </is>
+      </c>
+      <c r="D102" t="n">
+        <v>228</v>
+      </c>
+      <c r="E102" t="n">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>2019-11-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>2019-07-15</t>
+        </is>
+      </c>
+      <c r="F104" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>2019-07-18</t>
+        </is>
+      </c>
+      <c r="F105" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>2019-07-21</t>
+        </is>
+      </c>
+      <c r="F106" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>2019-07-24</t>
+        </is>
+      </c>
+      <c r="F107" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>2019-07-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>2019-07-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>2019-08-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>2019-08-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>2019-08-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>2019-08-11</t>
+        </is>
+      </c>
+      <c r="F113" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>2019-08-14</t>
+        </is>
+      </c>
+      <c r="F114" t="n">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>2019-08-15</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>2019-08-01</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>2019-08-04</t>
+        </is>
+      </c>
+      <c r="D117" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>2019-08-07</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>2019-08-10</t>
+        </is>
+      </c>
+      <c r="D119" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>2019-08-13</t>
+        </is>
+      </c>
+      <c r="D120" t="n">
+        <v>410</v>
+      </c>
+      <c r="F120" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>2019-08-16</t>
+        </is>
+      </c>
+      <c r="D121" t="n">
+        <v>410</v>
+      </c>
+      <c r="F121" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>2019-08-19</t>
+        </is>
+      </c>
+      <c r="D122" t="n">
+        <v>410</v>
+      </c>
+      <c r="F122" t="n">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>2019-08-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>2019-08-25</t>
+        </is>
+      </c>
+      <c r="F124" t="n">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>2019-08-28</t>
+        </is>
+      </c>
+      <c r="F125" t="n">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>2019-08-31</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>